<commit_message>
Updated June schedule manually
</commit_message>
<xml_diff>
--- a/schedule_2025_6.xlsx
+++ b/schedule_2025_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujjawal/Probe/doctor-sched/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CD869A-EAF2-F043-A7F5-F8A5477EA7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B16F0E-B23D-004A-811B-D230ED0BBA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,9 +656,9 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="185" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="222" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,10 +702,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>

</xml_diff>